<commit_message>
Tests with width search
</commit_message>
<xml_diff>
--- a/Trabalho 1/quebra_cabeca_8_pecas/Experiments.xlsx
+++ b/Trabalho 1/quebra_cabeca_8_pecas/Experiments.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="15">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -260,7 +260,203 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="98">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3747,6 +3943,18 @@
                 <c:pt idx="2">
                   <c:v>190635</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>1527</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17733</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>184126</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>181561</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3908,6 +4116,18 @@
                 <c:pt idx="2">
                   <c:v>11</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4094,6 +4314,18 @@
                       <c:pt idx="2">
                         <c:v>0</c:v>
                       </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4266,6 +4498,18 @@
                       </c:pt>
                       <c:pt idx="2" formatCode="General">
                         <c:v>13.002000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>0.72499999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>8.7750000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>89.37</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>169.761</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4709,6 +4953,18 @@
                 <c:pt idx="3" formatCode="General">
                   <c:v>510.63499999999999</c:v>
                 </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.72499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>8.7750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>89.37</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>169.761</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4919,6 +5175,18 @@
                       <c:pt idx="3">
                         <c:v>0</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -5128,9 +5396,6 @@
                       <c:pt idx="7">
                         <c:v>100000</c:v>
                       </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1000000</c:v>
-                      </c:pt>
                       <c:pt idx="9">
                         <c:v>100000</c:v>
                       </c:pt>
@@ -5340,6 +5605,18 @@
                       <c:pt idx="3">
                         <c:v>1850203</c:v>
                       </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1527</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>17733</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>184126</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>181561</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -5536,6 +5813,18 @@
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>16</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -8303,7 +8592,7 @@
   <dimension ref="B2:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8828,138 +9117,138 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E16:F27 E8 F8:F10 E3:F3">
-    <cfRule type="cellIs" dxfId="69" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="37" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="38" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="67" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="35" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="65" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="33" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="34" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="63" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="31" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="32" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="61" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="29" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="30" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12 F12:F14">
-    <cfRule type="cellIs" dxfId="59" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="27" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="28" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="57" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="25" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="26" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="55" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="23" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="24" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="53" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="21" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="22" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="51" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="19" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F5">
-    <cfRule type="cellIs" dxfId="49" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="17" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="18" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="47" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="15" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="45" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="11" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="12" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="41" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="9" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="10" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8974,19 +9263,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="2"/>
@@ -9155,14 +9444,22 @@
       <c r="D8" s="8">
         <v>100</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="F8" s="8">
         <f t="shared" ref="F8:F15" si="1">C8</f>
         <v>1000</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="G8" s="8">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1527</v>
+      </c>
+      <c r="I8" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
@@ -9174,14 +9471,22 @@
       <c r="D9" s="8">
         <v>100</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="F9" s="8">
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="G9" s="8">
+        <v>8.7750000000000004</v>
+      </c>
+      <c r="H9" s="8">
+        <v>17733</v>
+      </c>
+      <c r="I9" s="8">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
@@ -9193,14 +9498,22 @@
       <c r="D10" s="8">
         <v>100</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="F10" s="8">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="G10" s="8">
+        <v>89.37</v>
+      </c>
+      <c r="H10" s="8">
+        <v>184126</v>
+      </c>
+      <c r="I10" s="8">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
@@ -9213,10 +9526,7 @@
         <v>100</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="8">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
-      </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -9231,14 +9541,22 @@
       <c r="D12" s="8">
         <v>250</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="F12" s="8">
-        <f t="shared" si="1"/>
+        <f>C12</f>
         <v>100000</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="G12" s="8">
+        <v>169.761</v>
+      </c>
+      <c r="H12" s="8">
+        <v>181561</v>
+      </c>
+      <c r="I12" s="8">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
@@ -9436,131 +9754,155 @@
       <c r="E32" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E16:F27 E8 F8:F10 E3:F3">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+  <conditionalFormatting sqref="E16:F27 F8:F10 E3:F3">
+    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12 F12:F14">
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+  <conditionalFormatting sqref="F13:F14">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F5">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F7">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates in the experimets results
</commit_message>
<xml_diff>
--- a/Trabalho 1/quebra_cabeca_8_pecas/Experiments.xlsx
+++ b/Trabalho 1/quebra_cabeca_8_pecas/Experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjanuzi\Desktop\si2018\Trabalho 1\quebra_cabeca_8_pecas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjanuzi\Desktop\drive\03.Mestrado\2018\Semestre 2\Sistemas Inteligentes\si2018\Trabalho 1\quebra_cabeca_8_pecas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,54 +300,18 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -414,7 +378,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -925,7 +888,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>0.112</c:v>
+                  <c:v>0.127</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
                   <c:v>1000</c:v>
@@ -1015,13 +978,13 @@
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="0%">
-                  <c:v>0.31</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>0.876</c:v>
+                  <c:v>0.86199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>857.83</c:v>
+                  <c:v>832.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1112,7 +1075,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>0.17199999999999999</c:v>
+                  <c:v>0.17799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
                   <c:v>1000</c:v>
@@ -1206,10 +1169,10 @@
                   <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>1.01</c:v>
+                  <c:v>1.0149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>955.82</c:v>
+                  <c:v>955.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1223,11 +1186,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198458656"/>
-        <c:axId val="198475736"/>
+        <c:axId val="179453080"/>
+        <c:axId val="179453472"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="198458656"/>
+        <c:axId val="179453080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1269,7 +1232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198475736"/>
+        <c:crossAx val="179453472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1277,7 +1240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198475736"/>
+        <c:axId val="179453472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1301,7 +1264,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198458656"/>
+        <c:crossAx val="179453080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1315,7 +1278,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1431,7 +1393,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1938,7 +1899,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>1.127</c:v>
+                  <c:v>1.272</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
                   <c:v>10000</c:v>
@@ -2028,13 +1989,13 @@
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="0%">
-                  <c:v>0.47</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>6.6559999999999997</c:v>
+                  <c:v>5.7350000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>5914.43</c:v>
+                  <c:v>5036.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2125,7 +2086,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>1.722</c:v>
+                  <c:v>1.7270000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
                   <c:v>10000</c:v>
@@ -2216,13 +2177,13 @@
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="0%">
-                  <c:v>0.35</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>8.51</c:v>
+                  <c:v>9.3089999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>7227.07</c:v>
+                  <c:v>7899.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2236,11 +2197,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198586896"/>
-        <c:axId val="199007312"/>
+        <c:axId val="179454256"/>
+        <c:axId val="179454648"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="198586896"/>
+        <c:axId val="179454256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2282,7 +2243,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199007312"/>
+        <c:crossAx val="179454648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2290,7 +2251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199007312"/>
+        <c:axId val="179454648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2314,7 +2275,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198586896"/>
+        <c:crossAx val="179454256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2328,7 +2289,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3813,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3967,9 +3927,18 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="F8" s="12">
+        <f>(F6-F4)/F4</f>
+        <v>10.19481981981982</v>
+      </c>
+      <c r="G8" s="12">
+        <f>(G6-G4)/G4</f>
+        <v>-0.47703454849654381</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" ref="G8:H8" si="0">(H6-H4)/H4</f>
+        <v>-6.4950000000000728E-3</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
@@ -3985,8 +3954,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
@@ -4099,8 +4067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4254,9 +4222,18 @@
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="F8" s="12">
+        <f>(F6-F4)/F4</f>
+        <v>9.4446742502585312</v>
+      </c>
+      <c r="G8" s="12">
+        <f>(G6-G4)/G4</f>
+        <v>-4.2143769181283902E-2</v>
+      </c>
+      <c r="H8" s="12">
+        <f>(H6-H4)/H4</f>
+        <v>0.49666666666666676</v>
+      </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
@@ -4275,7 +4252,10 @@
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4">
+        <f>POWER(3,H4)</f>
+        <v>19683</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
@@ -4285,7 +4265,10 @@
       <c r="D11" s="4"/>
       <c r="E11" s="1"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4">
+        <f>POWER(3,H6)</f>
+        <v>2671919.0789592504</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
@@ -4296,22 +4279,30 @@
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
+      <c r="G13" s="2">
+        <f>G11-G10</f>
+        <v>2652236.0789592504</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E15" s="3"/>
+      <c r="G15" s="12">
+        <f>G13/G10</f>
+        <v>134.74755265758523</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E16" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E7:F11">
-    <cfRule type="cellIs" dxfId="3" priority="48" operator="equal">
+  <conditionalFormatting sqref="E7:F7 E9:F11 E8">
+    <cfRule type="cellIs" dxfId="1" priority="48" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="49" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4338,7 +4329,7 @@
   <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B14" activeCellId="5" sqref="A4:XFD4 A6:XFD6 A8:XFD8 A10:XFD10 A12:XFD12 A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4395,14 +4386,14 @@
         <v>0</v>
       </c>
       <c r="F3" s="9">
-        <v>0.112</v>
+        <v>0.127</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9">
         <v>1000</v>
       </c>
       <c r="I3" s="9">
-        <v>7.93</v>
+        <v>7.92</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -4419,14 +4410,14 @@
         <v>0</v>
       </c>
       <c r="F4" s="9">
-        <v>1.127</v>
+        <v>1.272</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9">
         <v>10000</v>
       </c>
       <c r="I4" s="9">
-        <v>7.98</v>
+        <v>8.16</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -4440,17 +4431,17 @@
         <v>250</v>
       </c>
       <c r="E5" s="10">
-        <v>0.31</v>
+        <v>0.37</v>
       </c>
       <c r="F5" s="9">
-        <v>0.876</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9">
-        <v>857.83</v>
+        <v>832.78</v>
       </c>
       <c r="I5" s="9">
-        <v>2.2200000000000002</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -4464,14 +4455,14 @@
         <v>250</v>
       </c>
       <c r="E6" s="10">
-        <v>0.47</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F6" s="9">
-        <v>6.6559999999999997</v>
+        <v>5.7350000000000003</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9">
-        <v>5914.43</v>
+        <v>5036.03</v>
       </c>
       <c r="I6" s="9">
         <v>2</v>
@@ -4491,7 +4482,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="9">
-        <v>0.17199999999999999</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9">
@@ -4515,14 +4506,14 @@
         <v>0</v>
       </c>
       <c r="F8" s="9">
-        <v>1.722</v>
+        <v>1.7270000000000001</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9">
         <v>10000</v>
       </c>
       <c r="I8" s="9">
-        <v>9.94</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
@@ -4539,14 +4530,14 @@
         <v>0.09</v>
       </c>
       <c r="F9" s="9">
-        <v>1.01</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9">
-        <v>955.82</v>
+        <v>955.32</v>
       </c>
       <c r="I9" s="9">
-        <v>3.58</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -4560,17 +4551,17 @@
         <v>250</v>
       </c>
       <c r="E10" s="10">
-        <v>0.35</v>
+        <v>0.26</v>
       </c>
       <c r="F10" s="9">
-        <v>8.51</v>
+        <v>9.3089999999999993</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9">
-        <v>7227.07</v>
+        <v>7899.41</v>
       </c>
       <c r="I10" s="9">
-        <v>2.66</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
@@ -4587,7 +4578,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="9">
-        <v>0.20100000000000001</v>
+        <v>0.19700000000000001</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9">
@@ -4611,7 +4602,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="9">
-        <v>2.0409999999999999</v>
+        <v>1.98</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9">
@@ -4632,14 +4623,14 @@
         <v>250</v>
       </c>
       <c r="E13" s="10">
-        <v>0.31</v>
+        <v>0.22</v>
       </c>
       <c r="F13" s="9">
-        <v>0.88200000000000001</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9">
-        <v>799.95</v>
+        <v>847.28</v>
       </c>
       <c r="I13" s="9">
         <v>5.32</v>
@@ -4656,17 +4647,17 @@
         <v>250</v>
       </c>
       <c r="E14" s="10">
-        <v>0.33</v>
+        <v>0.26</v>
       </c>
       <c r="F14" s="9">
-        <v>8.3170000000000002</v>
+        <v>8.9550000000000001</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9">
-        <v>6793.86</v>
+        <v>7483.88</v>
       </c>
       <c r="I14" s="9">
-        <v>5.0199999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>